<commit_message>
change process CDM mapping
</commit_message>
<xml_diff>
--- a/CDM/Dash_eng/join_table/join_table_condition.xlsx
+++ b/CDM/Dash_eng/join_table/join_table_condition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sungjoo\Desktop\sungjoo\09.분석업무\04.CDM_Dashboard\03.질지표\03.분석\_data\join_table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsj28\Desktop\CDM-dash\응급실\_data\join_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909F369B-B881-486B-957C-AD2919C1C96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73F7688-D6FD-4464-866E-B78E2D24DF77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9DD6E51-E791-453C-BE90-2E46F74872A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9DD6E51-E791-453C-BE90-2E46F74872A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>condition_source_value</t>
   </si>
@@ -41,16 +41,27 @@
   <si>
     <t>condition_concept_id</t>
   </si>
+  <si>
+    <t>DOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -398,16 +409,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,18 +430,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>63238001</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>4269348</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>4269348</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>